<commit_message>
Add User Create Page
</commit_message>
<xml_diff>
--- a/Item_Definition.xlsx
+++ b/Item_Definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\POS_System_Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621FEE9E-357B-420F-A398-CADC0BB7C7A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{344E6175-B330-45FB-B725-808428B772B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CB71EF2B-E407-4C0F-8146-21B4609D5872}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="40">
   <si>
     <t>Menu Code</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>Permission Code</t>
+  </si>
+  <si>
+    <t>Permission Name</t>
   </si>
 </sst>
 </file>
@@ -514,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8867269-F257-487A-94BD-145A2348EB9A}">
-  <dimension ref="A2:E22"/>
+  <dimension ref="A2:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,9 +530,10 @@
     <col min="3" max="3" width="33" customWidth="1"/>
     <col min="4" max="4" width="36.6640625" customWidth="1"/>
     <col min="5" max="5" width="36.44140625" customWidth="1"/>
+    <col min="6" max="6" width="29.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -545,8 +549,11 @@
       <c r="E2" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -562,8 +569,11 @@
       <c r="E4" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -579,8 +589,11 @@
       <c r="E6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>6</v>
       </c>
@@ -590,8 +603,11 @@
       <c r="E7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>8</v>
       </c>
@@ -601,8 +617,11 @@
       <c r="E8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>9</v>
       </c>
@@ -612,8 +631,11 @@
       <c r="E9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>15</v>
       </c>
@@ -623,8 +645,11 @@
       <c r="E10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -640,8 +665,11 @@
       <c r="E12" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C13" t="s">
         <v>6</v>
       </c>
@@ -651,8 +679,11 @@
       <c r="E13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C14" t="s">
         <v>8</v>
       </c>
@@ -662,8 +693,11 @@
       <c r="E14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C15" t="s">
         <v>9</v>
       </c>
@@ -673,8 +707,11 @@
       <c r="E15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C16" t="s">
         <v>15</v>
       </c>
@@ -684,8 +721,11 @@
       <c r="E16" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>25</v>
       </c>
@@ -701,8 +741,11 @@
       <c r="E18" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C19" t="s">
         <v>6</v>
       </c>
@@ -712,8 +755,11 @@
       <c r="E19" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C20" t="s">
         <v>8</v>
       </c>
@@ -723,8 +769,11 @@
       <c r="E20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C21" t="s">
         <v>9</v>
       </c>
@@ -734,8 +783,11 @@
       <c r="E21" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>15</v>
       </c>
@@ -744,6 +796,9 @@
       </c>
       <c r="E22" t="s">
         <v>29</v>
+      </c>
+      <c r="F22" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>